<commit_message>
Added decimal support for getStrExcel method if != .00
</commit_message>
<xml_diff>
--- a/src/main/resources/Test.xlsx
+++ b/src/main/resources/Test.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/danielcallif/Desktop/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/danielcallif/Development/ExcelReader/src/main/resources/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{95DEFDD7-18C7-3E41-9ED6-C791D4783AD1}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EBB6D35B-170F-8547-B94E-CC0E775F2395}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="380" yWindow="440" windowWidth="28040" windowHeight="15960" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -44,6 +44,9 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="1">
+    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
+  </numFmts>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -73,8 +76,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -389,15 +393,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D2"/>
+  <dimension ref="A1:E2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F8" sqref="F8"/>
+      <selection activeCell="E1" sqref="E1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -410,8 +414,11 @@
       <c r="D1">
         <v>123456</v>
       </c>
+      <c r="E1" s="1">
+        <v>100.75</v>
+      </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>3</v>
       </c>

</xml_diff>

<commit_message>
Added get Bool from cell with test
</commit_message>
<xml_diff>
--- a/src/main/resources/Test.xlsx
+++ b/src/main/resources/Test.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/danielcallif/Development/ExcelReader/src/main/resources/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EBB6D35B-170F-8547-B94E-CC0E775F2395}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{35AF3AF9-3728-974A-8356-475EC3FB5A4D}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="380" yWindow="440" windowWidth="28040" windowHeight="15960" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -396,7 +396,7 @@
   <dimension ref="A1:E2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E1" sqref="E1"/>
+      <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -431,6 +431,9 @@
       <c r="D2" t="b">
         <v>1</v>
       </c>
+      <c r="E2" t="b">
+        <v>0</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>